<commit_message>
[#7636] fix diary excel
</commit_message>
<xml_diff>
--- a/storage/app/excel/child_diary.xlsx
+++ b/storage/app/excel/child_diary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>001-保育園</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>保育日誌</t>
+  </si>
+  <si>
+    <t>天気：</t>
   </si>
   <si>
     <t>0歳児クラス</t>
@@ -77,10 +80,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -118,14 +121,36 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,19 +164,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -171,17 +187,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -192,46 +201,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -246,10 +218,41 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -300,43 +303,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -348,25 +447,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -378,37 +477,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,74 +487,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -545,21 +548,6 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFFFFFFF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -650,15 +638,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -704,6 +683,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -727,31 +726,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -761,134 +749,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -940,8 +928,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -949,46 +946,43 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1313,7 +1307,7 @@
   <dimension ref="A1:AD47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="J3" sqref="J3:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1350,7 +1344,7 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" ht="15.75" spans="1:30">
+    <row r="2" spans="1:30">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1382,7 +1376,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" ht="15.75" spans="1:30">
+    <row r="3" spans="1:30">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
@@ -1394,7 +1388,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="J3" s="17"/>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
@@ -1404,21 +1398,21 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="18" t="s">
+      <c r="T3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="U3" s="19"/>
-      <c r="V3" s="18" t="s">
+      <c r="U3" s="21"/>
+      <c r="V3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
-      <c r="Y3" s="20"/>
-      <c r="Z3" s="19"/>
-      <c r="AA3" s="18" t="s">
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="AB3" s="19"/>
+      <c r="AB3" s="21"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
@@ -1434,25 +1428,27 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="J4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="21"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="21"/>
-      <c r="AB4" s="22"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="24"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
@@ -1476,15 +1472,15 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="24"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="26"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="24"/>
-      <c r="AB5" s="25"/>
+      <c r="Z5" s="27"/>
+      <c r="AA5" s="26"/>
+      <c r="AB5" s="27"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
@@ -1508,15 +1504,15 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="26"/>
-      <c r="W6" s="28"/>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="28"/>
-      <c r="Z6" s="27"/>
-      <c r="AA6" s="26"/>
-      <c r="AB6" s="27"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="30"/>
+      <c r="X6" s="30"/>
+      <c r="Y6" s="30"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="28"/>
+      <c r="AB6" s="29"/>
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
@@ -1524,7 +1520,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1621,17 +1617,17 @@
     <row r="10" spans="1:30">
       <c r="A10" s="1"/>
       <c r="B10" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -1644,7 +1640,7 @@
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
@@ -1861,13 +1857,13 @@
     <row r="17" spans="1:30">
       <c r="A17" s="1"/>
       <c r="B17" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -1879,20 +1875,20 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
-      <c r="Q17" s="29" t="s">
-        <v>13</v>
+      <c r="Q17" s="31" t="s">
+        <v>14</v>
       </c>
-      <c r="R17" s="30"/>
-      <c r="S17" s="30"/>
-      <c r="T17" s="30"/>
-      <c r="U17" s="30"/>
-      <c r="V17" s="30"/>
-      <c r="W17" s="30"/>
-      <c r="X17" s="30"/>
-      <c r="Y17" s="30"/>
-      <c r="Z17" s="30"/>
-      <c r="AA17" s="30"/>
-      <c r="AB17" s="31"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="32"/>
+      <c r="Y17" s="32"/>
+      <c r="Z17" s="32"/>
+      <c r="AA17" s="32"/>
+      <c r="AB17" s="33"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
@@ -2027,7 +2023,7 @@
     <row r="22" spans="1:30">
       <c r="A22" s="1"/>
       <c r="B22" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2054,7 +2050,7 @@
       <c r="Y22" s="13"/>
       <c r="Z22" s="13"/>
       <c r="AA22" s="13"/>
-      <c r="AB22" s="32"/>
+      <c r="AB22" s="34"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="1"/>
     </row>
@@ -2086,14 +2082,14 @@
       <c r="Y23" s="15"/>
       <c r="Z23" s="15"/>
       <c r="AA23" s="15"/>
-      <c r="AB23" s="33"/>
+      <c r="AB23" s="35"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="1"/>
     </row>
     <row r="24" spans="1:30">
       <c r="A24" s="1"/>
       <c r="B24" s="16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -2120,7 +2116,7 @@
       <c r="Y24" s="13"/>
       <c r="Z24" s="13"/>
       <c r="AA24" s="13"/>
-      <c r="AB24" s="32"/>
+      <c r="AB24" s="34"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="1"/>
     </row>
@@ -2152,7 +2148,7 @@
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
       <c r="AA25" s="15"/>
-      <c r="AB25" s="33"/>
+      <c r="AB25" s="35"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="1"/>
     </row>
@@ -2223,7 +2219,7 @@
     <row r="28" spans="1:30">
       <c r="A28" s="1"/>
       <c r="B28" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -2513,7 +2509,7 @@
     <row r="37" spans="1:30">
       <c r="A37" s="1"/>
       <c r="B37" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -2865,11 +2861,13 @@
       <c r="AD47" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="31">
     <mergeCell ref="C3:E3"/>
+    <mergeCell ref="J3:M3"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="V3:Z3"/>
     <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="K4:M4"/>
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="F10:P10"/>
     <mergeCell ref="Q10:AB10"/>

</xml_diff>

<commit_message>
fix child diary exel
</commit_message>
<xml_diff>
--- a/storage/app/excel/child_diary.xlsx
+++ b/storage/app/excel/child_diary.xlsx
@@ -80,10 +80,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -128,7 +128,53 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -143,44 +189,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,7 +212,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,48 +257,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,187 +303,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,11 +629,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -653,17 +659,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -679,6 +688,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -702,36 +726,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -749,130 +749,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -899,7 +899,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -914,16 +914,16 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -980,10 +980,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1306,8 +1306,8 @@
   <sheetPr/>
   <dimension ref="A1:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:M3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>